<commit_message>
Adding threading and sheetoperator workarround
</commit_message>
<xml_diff>
--- a/Web.xlsx
+++ b/Web.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView activeTab="0" windowHeight="11160" windowWidth="20730" xWindow="-120" yWindow="-120"/>
   </bookViews>
   <sheets>
     <sheet name="Web" sheetId="2" r:id="rId1"/>
@@ -22,12 +22,23 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="8" mc:Ignorable="x14ac">
+  <numFmts count="8">
+    <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);(&quot;$&quot;#,##0)"/>
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red](&quot;$&quot;#,##0)"/>
+    <numFmt numFmtId="7" formatCode="&quot;$&quot;#,##0.00_);(&quot;$&quot;#,##0.00)"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red](&quot;$&quot;#,##0.00)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* (#,##0);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* (#,##0);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* (#,##0.00);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* (#,##0.00);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="1">
     <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="10"/>
     </font>
   </fonts>
   <fills count="2">
@@ -40,15 +51,25 @@
   </fills>
   <borders count="1">
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -11058,14 +11079,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L291"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A256" workbookViewId="0">
-      <selection activeCell="A292" sqref="A292"/>
+    <sheetView topLeftCell="A256" workbookViewId="0" tabSelected="1">
+      <selection pane="topLeft" activeCell="H285" sqref="H285"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12"/>
   <cols>
     <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.140625" bestFit="1" customWidth="1"/>
@@ -11104,9 +11124,8 @@
         <f>'[1]Resum ind.'!C4</f>
         <v>Oju Peligru</v>
       </c>
-      <c r="D2">
-        <f>'[1]Resum ind.'!D4</f>
-        <v>90</v>
+      <c r="D2" s="0">
+        <v>1</v>
       </c>
       <c r="E2" t="str">
         <f>'[1]Resum ind.'!E4</f>
@@ -11124,9 +11143,8 @@
         <f>'[1]Resum ind.'!H4</f>
         <v/>
       </c>
-      <c r="I2">
-        <f>'[1]Resum ind.'!I4</f>
-        <v>810</v>
+      <c r="I2" s="0">
+        <v>1</v>
       </c>
       <c r="J2">
         <f>'[1]Resum ind.'!J4</f>
@@ -24872,9 +24890,8 @@
         <f>'[1]Resum equips'!G38</f>
         <v/>
       </c>
-      <c r="H284">
-        <f>'[1]Resum equips'!H38</f>
-        <v>158</v>
+      <c r="H284" s="0">
+        <v>300</v>
       </c>
       <c r="I284">
         <f>'[1]Resum equips'!I38</f>

</xml_diff>